<commit_message>
fixed the mine file to get rid of paths double wide
</commit_message>
<xml_diff>
--- a/Mine2.xlsx
+++ b/Mine2.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Taylan\Documents\Programming\Java\workspace\FinalProject\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3420" windowWidth="30040" windowHeight="16140"/>
+    <workbookView xWindow="3900" yWindow="3420" windowWidth="30045" windowHeight="16140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,7 +68,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,6 +160,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -450,10 +458,10 @@
   <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="AF12" sqref="AF12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="3.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="3.875" defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" t="s">
@@ -663,11 +671,11 @@
       <c r="D4" t="s">
         <v>0</v>
       </c>
-      <c r="E4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>1</v>
+      <c r="E4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>1</v>
@@ -728,11 +736,11 @@
       <c r="D5" t="s">
         <v>0</v>
       </c>
-      <c r="E5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>1</v>
+      <c r="E5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>1</v>
@@ -793,11 +801,11 @@
       <c r="D6" t="s">
         <v>0</v>
       </c>
-      <c r="E6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>10</v>
+      <c r="E6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>0</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>1</v>
@@ -1018,8 +1026,8 @@
       <c r="N9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O9" s="1" t="s">
-        <v>1</v>
+      <c r="O9" t="s">
+        <v>0</v>
       </c>
       <c r="P9" t="s">
         <v>0</v>
@@ -1834,7 +1842,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1851,7 +1859,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>